<commit_message>
add checks on database
</commit_message>
<xml_diff>
--- a/HybridCars_2017.xlsx
+++ b/HybridCars_2017.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dane/Dropbox/Data/EV/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dane/src/evsales/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F6A4FB-2431-2940-87ED-2E704AF04DC3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="13720" windowWidth="20060" windowHeight="12780" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1320" yWindow="13720" windowWidth="20060" windowHeight="12780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -63,7 +62,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -375,11 +374,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -801,7 +800,7 @@
         <v>34</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11">
         <v>52</v>

</xml_diff>